<commit_message>
Remove add bulk user into group at group management. Filter user by group in user management
</commit_message>
<xml_diff>
--- a/public/excel_template/User/Bulk_Update.xlsx
+++ b/public/excel_template/User/Bulk_Update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user'\Documents\AWC_LMS\Code\frontend\public\excel_template\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CF9ACE-B1E7-462A-A2C1-BA043FA6DD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3755AC-3B7F-487C-A01C-6539D03D6662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BBD93479-F0D6-40A1-8937-1DFA47C5B9A3}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>